<commit_message>
add data integration code for CER datasets
</commit_message>
<xml_diff>
--- a/DATA2_LRET/Data Dictionary.xlsx
+++ b/DATA2_LRET/Data Dictionary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rengga\USyd\All Materials\Courses Materials\Semester II\1. Data Engineering\data_engineering\DATA2_LRET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934237CC-F866-43AD-96DD-E52CBD79BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AC1348-8CA3-456C-A231-424ED9BF4A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{0EB6E0F8-2826-4008-B437-EA8333107275}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0EB6E0F8-2826-4008-B437-EA8333107275}"/>
   </bookViews>
   <sheets>
-    <sheet name="Approved" sheetId="2" r:id="rId1"/>
-    <sheet name="Committed" sheetId="1" r:id="rId2"/>
+    <sheet name="CER_Approved" sheetId="2" r:id="rId1"/>
+    <sheet name="CER_Committed" sheetId="1" r:id="rId2"/>
+    <sheet name="CER_Probable" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Column</t>
   </si>
@@ -185,6 +186,9 @@
   </si>
   <si>
     <t>committed_month</t>
+  </si>
+  <si>
+    <t>Status of the project (probable)</t>
   </si>
 </sst>
 </file>
@@ -243,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,12 +266,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -588,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCD5208-ED88-4FC8-B28A-CEE6D0B24A0D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -762,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549929FF-083A-4A74-9B2D-6A7D35F0635C}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -877,37 +875,160 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E4F0A8-2471-4BE3-91F8-BC1C9DC4CFBA}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="64.77734375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>